<commit_message>
updating enter data into website
</commit_message>
<xml_diff>
--- a/Enter Excel Data into Website/Project_Notebook.xlsx
+++ b/Enter Excel Data into Website/Project_Notebook.xlsx
@@ -1602,4 +1602,1766 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=Project_Notebook/[Content_Types].xml><?xml version="1.0" encoding="utf-8"?>
+<Types xmlns="http://schemas.openxmlformats.org/package/2006/content-types">
+  <Default Extension="bin" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.printerSettings"/>
+  <Default Extension="rels" ContentType="application/vnd.openxmlformats-package.relationships+xml"/>
+  <Default Extension="xml" ContentType="application/xml"/>
+  <Override PartName="/xl/workbook.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.sheet.main+xml"/>
+  <Override PartName="/xl/worksheets/sheet1.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.worksheet+xml"/>
+  <Override PartName="/xl/worksheets/sheet2.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.worksheet+xml"/>
+  <Override PartName="/xl/worksheets/sheet3.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.worksheet+xml"/>
+  <Override PartName="/xl/worksheets/sheet4.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.worksheet+xml"/>
+  <Override PartName="/xl/worksheets/sheet5.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.worksheet+xml"/>
+  <Override PartName="/xl/theme/theme1.xml" ContentType="application/vnd.openxmlformats-officedocument.theme+xml"/>
+  <Override PartName="/xl/styles.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.styles+xml"/>
+  <Override PartName="/xl/sharedStrings.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.sharedStrings+xml"/>
+  <Override PartName="/xl/metadata.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.sheetMetadata+xml"/>
+  <Override PartName="/xl/calcChain.xml" ContentType="application/vnd.openxmlformats-officedocument.spreadsheetml.calcChain+xml"/>
+  <Override PartName="/docProps/core.xml" ContentType="application/vnd.openxmlformats-package.core-properties+xml"/>
+  <Override PartName="/docProps/app.xml" ContentType="application/vnd.openxmlformats-officedocument.extended-properties+xml"/>
+</Types>
+</file>
+
+<file path=Project_Notebook/docProps/app.xml><?xml version="1.0" encoding="utf-8"?>
+<Properties xmlns="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <Application>Microsoft Excel</Application>
+  <DocSecurity>0</DocSecurity>
+  <ScaleCrop>false</ScaleCrop>
+  <HeadingPairs>
+    <vt:vector size="4" baseType="variant">
+      <vt:variant>
+        <vt:lpstr>Worksheets</vt:lpstr>
+      </vt:variant>
+      <vt:variant>
+        <vt:i4>5</vt:i4>
+      </vt:variant>
+      <vt:variant>
+        <vt:lpstr>Named Ranges</vt:lpstr>
+      </vt:variant>
+      <vt:variant>
+        <vt:i4>38</vt:i4>
+      </vt:variant>
+    </vt:vector>
+  </HeadingPairs>
+  <TitlesOfParts>
+    <vt:vector size="43" baseType="lpstr">
+      <vt:lpstr>Scratchpad</vt:lpstr>
+      <vt:lpstr>Date</vt:lpstr>
+      <vt:lpstr>Text</vt:lpstr>
+      <vt:lpstr>Number</vt:lpstr>
+      <vt:lpstr>File</vt:lpstr>
+      <vt:lpstr>CleanNumber</vt:lpstr>
+      <vt:lpstr>Contains</vt:lpstr>
+      <vt:lpstr>Date</vt:lpstr>
+      <vt:lpstr>DatePlusDays</vt:lpstr>
+      <vt:lpstr>DatePlusWorkingDays</vt:lpstr>
+      <vt:lpstr>DateText</vt:lpstr>
+      <vt:lpstr>Days</vt:lpstr>
+      <vt:lpstr>FileExtension</vt:lpstr>
+      <vt:lpstr>FileName</vt:lpstr>
+      <vt:lpstr>FileNameNoExtension</vt:lpstr>
+      <vt:lpstr>FirstName</vt:lpstr>
+      <vt:lpstr>Folder</vt:lpstr>
+      <vt:lpstr>FullFileName</vt:lpstr>
+      <vt:lpstr>Int</vt:lpstr>
+      <vt:lpstr>LastMonthEndDate</vt:lpstr>
+      <vt:lpstr>LastMonthStartDate</vt:lpstr>
+      <vt:lpstr>LastName</vt:lpstr>
+      <vt:lpstr>LastWeekFriday</vt:lpstr>
+      <vt:lpstr>LastWeekMonday</vt:lpstr>
+      <vt:lpstr>LastWeekSunday</vt:lpstr>
+      <vt:lpstr>Length</vt:lpstr>
+      <vt:lpstr>LowerCase</vt:lpstr>
+      <vt:lpstr>Number</vt:lpstr>
+      <vt:lpstr>NumberText</vt:lpstr>
+      <vt:lpstr>ReformattedDate</vt:lpstr>
+      <vt:lpstr>ReformattedFileName</vt:lpstr>
+      <vt:lpstr>ReformattedNumber</vt:lpstr>
+      <vt:lpstr>Replace</vt:lpstr>
+      <vt:lpstr>Result</vt:lpstr>
+      <vt:lpstr>Search</vt:lpstr>
+      <vt:lpstr>Text</vt:lpstr>
+      <vt:lpstr>ThisMonthFirstWorkingDay</vt:lpstr>
+      <vt:lpstr>ThisMonthLastWorkingDay</vt:lpstr>
+      <vt:lpstr>Today</vt:lpstr>
+      <vt:lpstr>Trimmed</vt:lpstr>
+      <vt:lpstr>TwoDecimals</vt:lpstr>
+      <vt:lpstr>UpperCase</vt:lpstr>
+      <vt:lpstr>YYYYMMDD</vt:lpstr>
+    </vt:vector>
+  </TitlesOfParts>
+  <Company/>
+  <LinksUpToDate>false</LinksUpToDate>
+  <SharedDoc>false</SharedDoc>
+  <HyperlinksChanged>false</HyperlinksChanged>
+  <AppVersion>16.0300</AppVersion>
+</Properties>
+</file>
+
+<file path=Project_Notebook/docProps/core.xml><?xml version="1.0" encoding="utf-8"?>
+<cp:coreProperties xmlns:cp="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:dcmitype="http://purl.org/dc/dcmitype/" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <dc:creator/>
+  <cp:lastModifiedBy/>
+  <dcterms:created xsi:type="dcterms:W3CDTF">2019-08-19T13:07:58Z</dcterms:created>
+  <dcterms:modified xsi:type="dcterms:W3CDTF">2020-02-11T10:44:07Z</dcterms:modified>
+</cp:coreProperties>
+</file>
+
+<file path=Project_Notebook/xl/calcChain.xml><?xml version="1.0" encoding="utf-8"?>
+<calcChain xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <c r="B4" i="4" l="1"/>
+  <c r="B6" i="4" s="1"/>
+  <c r="B5" i="4" l="1"/>
+  <c r="F5" i="3"/>
+  <c r="F6" i="3"/>
+  <c r="F7" i="3"/>
+  <c r="F8" i="3"/>
+  <c r="F4" i="3"/>
+  <c r="B14" i="5" l="1"/>
+  <c r="B10" i="5" l="1"/>
+  <c r="B7" i="5"/>
+  <c r="B15" i="3"/>
+  <c r="B14" i="3" s="1"/>
+  <c r="B8" i="5" l="1"/>
+  <c r="B9" i="5" s="1"/>
+  <c r="B14" i="4"/>
+  <c r="B10" i="1"/>
+  <c r="B21" i="1" l="1"/>
+  <c r="C21" i="1" s="1"/>
+  <c r="D21" i="1" s="1"/>
+  <c r="B3" i="1"/>
+  <c r="B7" i="1" s="1"/>
+  <c r="B12" i="3"/>
+  <c r="B11" i="3"/>
+  <c r="B7" i="3"/>
+  <c r="B6" i="3"/>
+  <c r="B5" i="3"/>
+  <c r="B4" i="3"/>
+  <c r="C13" i="1"/>
+  <c r="B13" i="1"/>
+  <c r="C12" i="1"/>
+  <c r="B12" i="1"/>
+  <c r="B11" i="1"/>
+  <c r="C11" i="1" s="1"/>
+  <c r="B8" i="1" l="1"/>
+  <c r="B6" i="1"/>
+  <c r="D11" i="1"/>
+  <c r="B24" i="1" a="1"/>
+  <c r="B24" i="1" s="1"/>
+  <c r="B22" i="1"/>
+  <c r="B23" i="1" s="1"/>
+  <c r="B25" i="1" l="1" a="1"/>
+  <c r="B25" i="1" s="1"/>
+  <c r="B26" i="1" a="1"/>
+  <c r="B26" i="1" s="1"/>
+  <c r="B28" i="1" l="1"/>
+</calcChain>
+</file>
+
+<file path=Project_Notebook/xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
+<file path=Project_Notebook/xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+  <si>
+    <t>Last month's dates (First and Last)</t>
+  </si>
+  <si>
+    <t>First / Last business day this month</t>
+  </si>
+  <si>
+    <t>Number Operations</t>
+  </si>
+  <si>
+    <t>Contains?</t>
+  </si>
+  <si>
+    <t>Date Operations</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>123.456,78</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>YMD</t>
+  </si>
+  <si>
+    <t>年</t>
+  </si>
+  <si>
+    <t>月</t>
+  </si>
+  <si>
+    <t>2008年12月31日 (水)</t>
+  </si>
+  <si>
+    <t>日</t>
+  </si>
+  <si>
+    <t>Date Format (YYYYMMDD)</t>
+  </si>
+  <si>
+    <t>Last week's dates (Monday, Friday, Sunday)</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Converts text to a number, in a locale-independent way</t>
+  </si>
+  <si>
+    <t>Converts text to a date, in a locale-independent way</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Calculated Values</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Separator</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Reformatted Date</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>Date (input)</t>
+  </si>
+  <si>
+    <t>1st token</t>
+  </si>
+  <si>
+    <t>2nd token</t>
+  </si>
+  <si>
+    <t>3rd token</t>
+  </si>
+  <si>
+    <t>Extracted Year</t>
+  </si>
+  <si>
+    <t>Extracted Month</t>
+  </si>
+  <si>
+    <t>Extracted Day</t>
+  </si>
+  <si>
+    <t>Decimal Separator</t>
+  </si>
+  <si>
+    <t>Group Separator</t>
+  </si>
+  <si>
+    <t>Reformatted Number</t>
+  </si>
+  <si>
+    <t>Number (input)</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>2 decimals</t>
+  </si>
+  <si>
+    <t>File name</t>
+  </si>
+  <si>
+    <t>File name no extension</t>
+  </si>
+  <si>
+    <t>File extension</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Trimmed</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Upper case</t>
+  </si>
+  <si>
+    <t>Lower case</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Replace</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Text Operations</t>
+  </si>
+  <si>
+    <t>Text (input)</t>
+  </si>
+  <si>
+    <t>Splits a full file name to get its folder and extension</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>C:\temp\Untitled Document.docx</t>
+  </si>
+  <si>
+    <t>Reformatted File Name:</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Date plus a number of days</t>
+  </si>
+  <si>
+    <t>Date plus a number of working days</t>
+  </si>
+  <si>
+    <t>Text to the left</t>
+  </si>
+  <si>
+    <t>Text to the right</t>
+  </si>
+  <si>
+    <t>Extracted text</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>John C. Doe</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>John C.</t>
+  </si>
+  <si>
+    <t>Cleaned Up</t>
+  </si>
+  <si>
+    <t>File System helpers</t>
+  </si>
+</sst>
+</file>
+
+<file path=Project_Notebook/xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="###,000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="11">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="39">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=Project_Notebook/xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
+<file path=Project_Notebook/xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Studio\Studio\UiPath.Studio.Plugin.Workflow\ProjectTemplates\Business Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F170A08E-9473-407E-9D66-3E9300B2639A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Scratchpad" sheetId="2" r:id="rId1"/>
+    <sheet name="Date" sheetId="1" r:id="rId2"/>
+    <sheet name="Text" sheetId="3" r:id="rId3"/>
+    <sheet name="Number" sheetId="4" r:id="rId4"/>
+    <sheet name="File" sheetId="5" r:id="rId5"/>
+  </sheets>
+  <definedNames>
+    <definedName name="CleanNumber">Number!$B$4</definedName>
+    <definedName name="Contains">Text!$B$12</definedName>
+    <definedName name="Date">Date!$B$3</definedName>
+    <definedName name="DatePlusDays">Date!$B$6</definedName>
+    <definedName name="DatePlusWorkingDays">Date!$B$7</definedName>
+    <definedName name="DateText">Date!$B$17</definedName>
+    <definedName name="Days">Date!$B$5</definedName>
+    <definedName name="FileExtension">File!$B$8</definedName>
+    <definedName name="FileName">File!$B$7</definedName>
+    <definedName name="FileNameNoExtension">File!$B$9</definedName>
+    <definedName name="FirstName">Text!$B$14</definedName>
+    <definedName name="Folder">File!$B$10</definedName>
+    <definedName name="FullFileName">File!$B$5</definedName>
+    <definedName name="Int">Number!$B$5</definedName>
+    <definedName name="LastMonthEndDate">Date!$C$12</definedName>
+    <definedName name="LastMonthStartDate">Date!$B$12</definedName>
+    <definedName name="LastName">Text!$B$15</definedName>
+    <definedName name="LastWeekFriday">Date!$C$11</definedName>
+    <definedName name="LastWeekMonday">Date!$B$11</definedName>
+    <definedName name="LastWeekSunday">Date!$D$11</definedName>
+    <definedName name="Length">Text!$B$5</definedName>
+    <definedName name="LowerCase">Text!$B$7</definedName>
+    <definedName name="Number">Number!$B$3</definedName>
+    <definedName name="NumberText">Number!$B$10</definedName>
+    <definedName name="ReformattedDate">Date!$B$28</definedName>
+    <definedName name="ReformattedFileName">File!$B$14</definedName>
+    <definedName name="ReformattedNumber">Number!$B$14</definedName>
+    <definedName name="Replace">Text!$B$10</definedName>
+    <definedName name="Result">Text!$B$11</definedName>
+    <definedName name="Search">Text!$B$9</definedName>
+    <definedName name="Text">Text!$B$3</definedName>
+    <definedName name="ThisMonthFirstWorkingDay">Date!$B$13</definedName>
+    <definedName name="ThisMonthLastWorkingDay">Date!$C$13</definedName>
+    <definedName name="Today">Date!$B$10</definedName>
+    <definedName name="Trimmed">Text!$B$4</definedName>
+    <definedName name="TwoDecimals">Number!$B$6</definedName>
+    <definedName name="UpperCase">Text!$B$6</definedName>
+    <definedName name="YYYYMMDD">Date!$B$8</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=Project_Notebook/xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88115396-113A-4E92-ABEE-648E1977C738}">
+  <dimension ref="D1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="30" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="31"/>
+    </row>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=Project_Notebook/xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53392D88-1157-4343-9701-AA198E0565D5}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="4" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2">
+        <f ca="1">TODAY()</f>
+        <v>43872</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="2">
+        <f ca="1">Date+Days</f>
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2">
+        <f ca="1">WORKDAY(Date, Days)</f>
+        <v>43881</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="str">
+        <f ca="1">TEXT(Date,"YYYYMMDD")</f>
+        <v>20200211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2">
+        <f ca="1">TODAY()</f>
+        <v>43872</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <f ca="1">TODAY()-WEEKDAY(TODAY(),2)-6</f>
+        <v>43864</v>
+      </c>
+      <c r="C11" s="2">
+        <f ca="1">LastWeekMonday+4</f>
+        <v>43868</v>
+      </c>
+      <c r="D11" s="2">
+        <f ca="1">LastWeekFriday+2</f>
+        <v>43870</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1)</f>
+        <v>43831</v>
+      </c>
+      <c r="C12" s="2">
+        <f ca="1">DATE(YEAR(TODAY()), MONTH(TODAY()), 0)</f>
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <f ca="1">WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1)</f>
+        <v>43864</v>
+      </c>
+      <c r="C13" s="2">
+        <f ca="1">WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1)</f>
+        <v>43889</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="6" t="str">
+        <f>LEFT(B17, FIND(B18, B17)-1)</f>
+        <v>2008</v>
+      </c>
+      <c r="C21" s="6" t="str">
+        <f>RIGHT(B17, LEN(B17)-LEN(B21)-1)</f>
+        <v>12月31日 (水)</v>
+      </c>
+      <c r="D21" s="7" t="str">
+        <f>IF(D18&lt;&gt;"", LEFT(C21, FIND(D18, C21)-1), C21)</f>
+        <v>12月31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="6" t="str">
+        <f>LEFT(C21, FIND(C18, C21)-1)</f>
+        <v>12</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="6" t="str">
+        <f>RIGHT(D21, LEN(D21)-LEN(B22)-1)</f>
+        <v>31</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="6" t="str" cm="1">
+        <f t="array" ref="B24">_xlfn.SWITCH(FIND("Y", B19), 1, B21, 2, B22, 3, B23)</f>
+        <v>2008</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="6" t="str" cm="1">
+        <f t="array" ref="B25">_xlfn.SWITCH(FIND("M", B19), 1, B21, 2, B22, 3, B23)</f>
+        <v>12</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="6" t="str" cm="1">
+        <f t="array" ref="B26">_xlfn.SWITCH(FIND("D", B19), 1, B21, 2, B22, 3, B23)</f>
+        <v>31</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="8">
+        <f>DATE(B24, B25, B26)</f>
+        <v>39813</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A15:D15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=Project_Notebook/xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7C60E3-5132-4EAF-A6AE-357FE13BC6C9}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="str">
+        <f>TRIM(B3)</f>
+        <v>John C. Doe</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="28" t="str">
+        <f>TRIM(MID(Text, FIND(D4,Text)+LEN(D4), IFERROR(FIND(IF(E4="",CHAR(10),E4),Text,FIND(D4,Text)+LEN(D4)),LEN(Text)+1)-FIND(D4,Text)-LEN(D4)))</f>
+        <v>C.</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <f>LEN(B3)</f>
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="28" t="str">
+        <f>TRIM(MID(Text, FIND(D5,Text)+LEN(D5), IFERROR(FIND(IF(E5="",CHAR(10),E5),Text,FIND(D5,Text)+LEN(D5)),LEN(Text)+1)-FIND(D5,Text)-LEN(D5)))</f>
+        <v>C. Doe</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="str">
+        <f>UPPER(B3)</f>
+        <v>JOHN C. DOE</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="28" t="str">
+        <f>TRIM(MID(Text, FIND(D6,Text)+LEN(D6), IFERROR(FIND(IF(E6="",CHAR(10),E6),Text,FIND(D6,Text)+LEN(D6)),LEN(Text)+1)-FIND(D6,Text)-LEN(D6)))</f>
+        <v>John C.</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="str">
+        <f>LOWER(B3)</f>
+        <v>john c. doe</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="28" t="str">
+        <f>TRIM(MID(Text, FIND(D7,Text)+LEN(D7), IFERROR(FIND(IF(E7="",CHAR(10),E7),Text,FIND(D7,Text)+LEN(D7)),LEN(Text)+1)-FIND(D7,Text)-LEN(D7)))</f>
+        <v>Doe</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="28" t="str">
+        <f>TRIM(MID(Text, FIND(D8,Text)+LEN(D8), IFERROR(FIND(IF(E8="",CHAR(10),E8),Text,FIND(D8,Text)+LEN(D8)),LEN(Text)+1)-FIND(D8,Text)-LEN(D8)))</f>
+        <v>John C. Doe</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="str">
+        <f>SUBSTITUTE(Text, B9, B10)</f>
+        <v>Mary C. Doe</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="b">
+        <f>IF(IFERROR(FIND(B9, Text), FALSE), TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="str">
+        <f>LEFT(Text, LEN(Text)-LEN(LastName)-1)</f>
+        <v>John C.</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(B3," ",REPT(" ",LEN(B3))),LEN(B3)))</f>
+        <v>Doe</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=Project_Notebook/xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C83CC8-3284-4752-8E92-8CBBD1003835}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="29">
+        <v>3.1415929999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="25">
+        <f>VALUE(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Number, CHAR(13), ""), CHAR(10), ""), CHAR(160), "")))</f>
+        <v>3.1415929999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <f>INT(CleanNumber)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <f>INT(CleanNumber*100)/100</f>
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="38"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="11">
+        <f>IF(B11&lt;&gt;"",IF(B12&lt;&gt;"",_xlfn.NUMBERVALUE(B10, B11, B12),_xlfn.NUMBERVALUE(B10, B11)),IF(B12&lt;&gt;"",_xlfn.NUMBERVALUE(B10,, B12),_xlfn.NUMBERVALUE(B10)))</f>
+        <v>123456.78</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=Project_Notebook/xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B15AA95-D2AA-4AD6-8E83-DBFAD20B8498}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="4" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="38"/>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="26"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="17" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(B5,"\",REPT(" ",LEN(B5))),LEN(B5)))</f>
+        <v>Untitled Document.docx</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="17" t="str">
+        <f>TRIM(RIGHT(SUBSTITUTE(B7,".",REPT(" ",LEN(B7))),LEN(B7)))</f>
+        <v>docx</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="17" t="str">
+        <f>LEFT(B7, LEN(B7)-LEN(B8)-1)</f>
+        <v>Untitled Document</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="18" t="str">
+        <f>LEFT(B5, LEN(B5)-LEN(B7))</f>
+        <v>C:\temp\</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="25" t="str">
+        <f>FileNameNoExtension &amp; "." &amp; FileExtension</f>
+        <v>Untitled Document.docx</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>